<commit_message>
Correccion borrar unidades en WC 2007
</commit_message>
<xml_diff>
--- a/resources/WC-2007/WC-2007.xlsx
+++ b/resources/WC-2007/WC-2007.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cp\Documents\GitHub\DecatlonEstadistics\resources\WC-2007\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cp/Documents/GitHub/DecatlonEstadistics/resources/WC-2007/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCE0E87-9BC7-46E5-8406-B1E60AE16A9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59A4823-AD7A-574B-9615-3DD0425C042B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{34DEB7DA-1114-4C00-A5A7-79B4D4252A4A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{34DEB7DA-1114-4C00-A5A7-79B4D4252A4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>Pos</t>
   </si>
@@ -162,556 +162,25 @@
     <t>ESP</t>
   </si>
   <si>
-    <t>11.04s</t>
-  </si>
-  <si>
-    <t>7.56m</t>
-  </si>
-  <si>
-    <t>15.92m</t>
-  </si>
-  <si>
-    <t>2.12m</t>
-  </si>
-  <si>
-    <t>48.80s</t>
-  </si>
-  <si>
-    <t>14.33s</t>
-  </si>
-  <si>
-    <t>48.75m</t>
-  </si>
-  <si>
-    <t>4.80m</t>
-  </si>
-  <si>
-    <t>71.18m</t>
-  </si>
-  <si>
     <t>JAM</t>
   </si>
   <si>
-    <t>10.62s</t>
-  </si>
-  <si>
-    <t>7.50m</t>
-  </si>
-  <si>
-    <t>17.32m</t>
-  </si>
-  <si>
-    <t>1.97m</t>
-  </si>
-  <si>
-    <t>47.48s</t>
-  </si>
-  <si>
-    <t>13.91s</t>
-  </si>
-  <si>
-    <t>52.36m</t>
-  </si>
-  <si>
-    <t>53.61m</t>
-  </si>
-  <si>
     <t>KAZ</t>
   </si>
   <si>
-    <t>10.70s</t>
-  </si>
-  <si>
-    <t>7.19m</t>
-  </si>
-  <si>
-    <t>16.08m</t>
-  </si>
-  <si>
-    <t>2.06m</t>
-  </si>
-  <si>
-    <t>47.44s</t>
-  </si>
-  <si>
-    <t>14.03s</t>
-  </si>
-  <si>
-    <t>48.95m</t>
-  </si>
-  <si>
-    <t>5.00m</t>
-  </si>
-  <si>
-    <t>59.84m</t>
-  </si>
-  <si>
-    <t>10.97s</t>
-  </si>
-  <si>
-    <t>7.25m</t>
-  </si>
-  <si>
-    <t>16.49m</t>
-  </si>
-  <si>
-    <t>50.00s</t>
-  </si>
-  <si>
-    <t>14.76s</t>
-  </si>
-  <si>
-    <t>48.62m</t>
-  </si>
-  <si>
-    <t>63.51m</t>
-  </si>
-  <si>
-    <t>11.12s</t>
-  </si>
-  <si>
-    <t>7.42m</t>
-  </si>
-  <si>
-    <t>14.12m</t>
-  </si>
-  <si>
-    <t>49.40s</t>
-  </si>
-  <si>
-    <t>14.51s</t>
-  </si>
-  <si>
-    <t>44.48m</t>
-  </si>
-  <si>
-    <t>5.30m</t>
-  </si>
-  <si>
-    <t>63.28m</t>
-  </si>
-  <si>
-    <t>10.80s</t>
-  </si>
-  <si>
-    <t>7.01m</t>
-  </si>
-  <si>
-    <t>16.16m</t>
-  </si>
-  <si>
-    <t>2.03m</t>
-  </si>
-  <si>
-    <t>48.42s</t>
-  </si>
-  <si>
-    <t>14.59s</t>
-  </si>
-  <si>
-    <t>49.76m</t>
-  </si>
-  <si>
-    <t>4.90m</t>
-  </si>
-  <si>
-    <t>57.75m</t>
-  </si>
-  <si>
-    <t>11.36s</t>
-  </si>
-  <si>
-    <t>7.13m</t>
-  </si>
-  <si>
-    <t>15.03m</t>
-  </si>
-  <si>
-    <t>2.00m</t>
-  </si>
-  <si>
-    <t>49.32s</t>
-  </si>
-  <si>
-    <t>14.36s</t>
-  </si>
-  <si>
-    <t>44.51m</t>
-  </si>
-  <si>
-    <t>65.74m</t>
-  </si>
-  <si>
     <t>CUB</t>
   </si>
   <si>
-    <t>10.73s</t>
-  </si>
-  <si>
-    <t>7.15m</t>
-  </si>
-  <si>
-    <t>14.94m</t>
-  </si>
-  <si>
-    <t>2.09m</t>
-  </si>
-  <si>
-    <t>49.25s</t>
-  </si>
-  <si>
-    <t>14.08s</t>
-  </si>
-  <si>
-    <t>42.91m</t>
-  </si>
-  <si>
-    <t>4.70m</t>
-  </si>
-  <si>
-    <t>68.74m</t>
-  </si>
-  <si>
-    <t>10.87s</t>
-  </si>
-  <si>
-    <t>7.17m</t>
-  </si>
-  <si>
-    <t>13.58m</t>
-  </si>
-  <si>
-    <t>48.58s</t>
-  </si>
-  <si>
-    <t>13.92s</t>
-  </si>
-  <si>
-    <t>41.28m</t>
-  </si>
-  <si>
-    <t>65.24m</t>
-  </si>
-  <si>
-    <t>10.95s</t>
-  </si>
-  <si>
-    <t>7.26m</t>
-  </si>
-  <si>
-    <t>14.81m</t>
-  </si>
-  <si>
-    <t>49.34s</t>
-  </si>
-  <si>
-    <t>15.10s</t>
-  </si>
-  <si>
-    <t>44.81m</t>
-  </si>
-  <si>
-    <t>5.20m</t>
-  </si>
-  <si>
-    <t>55.96m</t>
-  </si>
-  <si>
-    <t>11.11s</t>
-  </si>
-  <si>
-    <t>7.35m</t>
-  </si>
-  <si>
-    <t>14.67m</t>
-  </si>
-  <si>
-    <t>1.88m</t>
-  </si>
-  <si>
-    <t>48.52s</t>
-  </si>
-  <si>
-    <t>14.77s</t>
-  </si>
-  <si>
-    <t>44.30m</t>
-  </si>
-  <si>
-    <t>4.30m</t>
-  </si>
-  <si>
-    <t>65.71m</t>
-  </si>
-  <si>
-    <t>11.44s</t>
-  </si>
-  <si>
-    <t>7.00m</t>
-  </si>
-  <si>
-    <t>15.13m</t>
-  </si>
-  <si>
-    <t>50.58s</t>
-  </si>
-  <si>
-    <t>14.82s</t>
-  </si>
-  <si>
-    <t>46.80m</t>
-  </si>
-  <si>
-    <t>59.63m</t>
-  </si>
-  <si>
-    <t>11.14s</t>
-  </si>
-  <si>
-    <t>6.86m</t>
-  </si>
-  <si>
-    <t>14.73m</t>
-  </si>
-  <si>
-    <t>49.02s</t>
-  </si>
-  <si>
-    <t>14.72s</t>
-  </si>
-  <si>
-    <t>43.70m</t>
-  </si>
-  <si>
-    <t>5.10m</t>
-  </si>
-  <si>
-    <t>56.01m</t>
-  </si>
-  <si>
     <t>BLR</t>
   </si>
   <si>
-    <t>11.29s</t>
-  </si>
-  <si>
-    <t>6.92m</t>
-  </si>
-  <si>
-    <t>15.98m</t>
-  </si>
-  <si>
-    <t>1.94m</t>
-  </si>
-  <si>
-    <t>51.16s</t>
-  </si>
-  <si>
-    <t>14.93s</t>
-  </si>
-  <si>
-    <t>44.86m</t>
-  </si>
-  <si>
-    <t>69.14m</t>
-  </si>
-  <si>
-    <t>10.67s</t>
-  </si>
-  <si>
-    <t>13.74m</t>
-  </si>
-  <si>
-    <t>1.85m</t>
-  </si>
-  <si>
-    <t>47.98s</t>
-  </si>
-  <si>
-    <t>15.02s</t>
-  </si>
-  <si>
-    <t>39.87m</t>
-  </si>
-  <si>
-    <t>57.73m</t>
-  </si>
-  <si>
-    <t>10.92s</t>
-  </si>
-  <si>
-    <t>14.26m</t>
-  </si>
-  <si>
-    <t>48.89s</t>
-  </si>
-  <si>
-    <t>37.07m</t>
-  </si>
-  <si>
-    <t>60.34m</t>
-  </si>
-  <si>
-    <t>11.17s</t>
-  </si>
-  <si>
-    <t>7.12m</t>
-  </si>
-  <si>
-    <t>13.29m</t>
-  </si>
-  <si>
-    <t>52.08s</t>
-  </si>
-  <si>
-    <t>14.75s</t>
-  </si>
-  <si>
-    <t>43.67m</t>
-  </si>
-  <si>
-    <t>56.69m</t>
-  </si>
-  <si>
-    <t>11.13s</t>
-  </si>
-  <si>
-    <t>7.43m</t>
-  </si>
-  <si>
-    <t>13.54m</t>
-  </si>
-  <si>
-    <t>50.37s</t>
-  </si>
-  <si>
-    <t>14.97s</t>
-  </si>
-  <si>
-    <t>41.69m</t>
-  </si>
-  <si>
-    <t>4.20m</t>
-  </si>
-  <si>
-    <t>56.28m</t>
-  </si>
-  <si>
     <t>JPN</t>
   </si>
   <si>
-    <t>11.05s</t>
-  </si>
-  <si>
-    <t>6.78m</t>
-  </si>
-  <si>
-    <t>11.92m</t>
-  </si>
-  <si>
-    <t>48.59s</t>
-  </si>
-  <si>
-    <t>15.53s</t>
-  </si>
-  <si>
-    <t>41.65m</t>
-  </si>
-  <si>
-    <t>59.59m</t>
-  </si>
-  <si>
-    <t>7.44m</t>
-  </si>
-  <si>
-    <t>13.23m</t>
-  </si>
-  <si>
-    <t>50.60s</t>
-  </si>
-  <si>
-    <t>15.17s</t>
-  </si>
-  <si>
-    <t>45.58m</t>
-  </si>
-  <si>
-    <t>4.40m</t>
-  </si>
-  <si>
-    <t>49.28m</t>
-  </si>
-  <si>
     <t>KOR</t>
   </si>
   <si>
-    <t>12.83m</t>
-  </si>
-  <si>
-    <t>1.91m</t>
-  </si>
-  <si>
-    <t>48.99s</t>
-  </si>
-  <si>
-    <t>14.89s</t>
-  </si>
-  <si>
-    <t>36.23m</t>
-  </si>
-  <si>
-    <t>44.79m</t>
-  </si>
-  <si>
-    <t>10.90s</t>
-  </si>
-  <si>
-    <t>15.18m</t>
-  </si>
-  <si>
-    <t>47.58s</t>
-  </si>
-  <si>
-    <t>14.71s</t>
-  </si>
-  <si>
-    <t>40.99m</t>
-  </si>
-  <si>
-    <t>NM</t>
-  </si>
-  <si>
-    <t>58.93m</t>
-  </si>
-  <si>
     <t>NOR</t>
-  </si>
-  <si>
-    <t>11.21s</t>
-  </si>
-  <si>
-    <t>6.93m</t>
-  </si>
-  <si>
-    <t>13.65m</t>
-  </si>
-  <si>
-    <t>1.82m</t>
-  </si>
-  <si>
-    <t>50.70s</t>
-  </si>
-  <si>
-    <t>27.24s</t>
-  </si>
-  <si>
-    <t>45.31m</t>
-  </si>
-  <si>
-    <t>4.50m</t>
-  </si>
-  <si>
-    <t>61.63m</t>
   </si>
   <si>
     <t>Maurice Smith</t>
@@ -1117,7 +586,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1415,25 +884,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97CAD70C-E319-4B1A-A34F-73775A44C87E}">
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="16" width="9.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="20" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="16" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" customWidth="1"/>
+    <col min="18" max="20" width="9.6640625" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" customWidth="1"/>
+    <col min="24" max="24" width="12.5" customWidth="1"/>
+    <col min="25" max="25" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1507,7 +976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -1523,56 +992,56 @@
       <c r="E2" s="19">
         <v>852</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>43</v>
+      <c r="F2" s="19">
+        <v>11.04</v>
       </c>
       <c r="G2" s="19">
         <v>950</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>44</v>
+      <c r="H2" s="18">
+        <v>7.56</v>
       </c>
       <c r="I2" s="18">
         <v>846</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>45</v>
+      <c r="J2" s="18">
+        <v>15.92</v>
       </c>
       <c r="K2" s="18">
         <v>915</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>46</v>
+      <c r="L2" s="18">
+        <v>2.12</v>
       </c>
       <c r="M2" s="18">
         <v>871</v>
       </c>
-      <c r="N2" s="18" t="s">
-        <v>47</v>
+      <c r="N2" s="18">
+        <v>48.8</v>
       </c>
       <c r="O2" s="18">
         <v>932</v>
       </c>
-      <c r="P2" s="18" t="s">
-        <v>48</v>
+      <c r="P2" s="18">
+        <v>14.33</v>
       </c>
       <c r="Q2" s="18">
         <v>844</v>
       </c>
-      <c r="R2" s="18" t="s">
-        <v>49</v>
+      <c r="R2" s="18">
+        <v>48.75</v>
       </c>
       <c r="S2" s="18">
         <v>849</v>
       </c>
-      <c r="T2" s="18" t="s">
-        <v>50</v>
+      <c r="T2" s="18">
+        <v>4.8</v>
       </c>
       <c r="U2" s="18">
         <v>907</v>
       </c>
-      <c r="V2" s="18" t="s">
-        <v>51</v>
+      <c r="V2" s="18">
+        <v>71.180000000000007</v>
       </c>
       <c r="W2" s="18">
         <v>710</v>
@@ -1581,15 +1050,15 @@
         <v>3.1865740740740743E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>227</v>
+        <v>50</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D3" s="19">
         <v>8644</v>
@@ -1597,56 +1066,56 @@
       <c r="E3" s="19">
         <v>947</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>53</v>
+      <c r="F3" s="19">
+        <v>10.62</v>
       </c>
       <c r="G3" s="19">
         <v>935</v>
       </c>
-      <c r="H3" s="18" t="s">
-        <v>54</v>
+      <c r="H3" s="18">
+        <v>7.5</v>
       </c>
       <c r="I3" s="18">
         <v>933</v>
       </c>
-      <c r="J3" s="18" t="s">
-        <v>55</v>
+      <c r="J3" s="18">
+        <v>17.32</v>
       </c>
       <c r="K3" s="18">
         <v>776</v>
       </c>
-      <c r="L3" s="18" t="s">
-        <v>56</v>
+      <c r="L3" s="18">
+        <v>1.97</v>
       </c>
       <c r="M3" s="18">
         <v>934</v>
       </c>
-      <c r="N3" s="18" t="s">
-        <v>57</v>
+      <c r="N3" s="18">
+        <v>47.48</v>
       </c>
       <c r="O3" s="18">
         <v>986</v>
       </c>
-      <c r="P3" s="18" t="s">
-        <v>58</v>
+      <c r="P3" s="18">
+        <v>13.91</v>
       </c>
       <c r="Q3" s="18">
         <v>920</v>
       </c>
-      <c r="R3" s="18" t="s">
-        <v>59</v>
+      <c r="R3" s="18">
+        <v>52.36</v>
       </c>
       <c r="S3" s="18">
         <v>849</v>
       </c>
-      <c r="T3" s="18" t="s">
-        <v>50</v>
+      <c r="T3" s="18">
+        <v>4.8</v>
       </c>
       <c r="U3" s="18">
         <v>642</v>
       </c>
-      <c r="V3" s="18" t="s">
-        <v>60</v>
+      <c r="V3" s="18">
+        <v>53.61</v>
       </c>
       <c r="W3" s="18">
         <v>722</v>
@@ -1655,15 +1124,15 @@
         <v>3.1657407407407402E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>228</v>
+        <v>51</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D4" s="19">
         <v>8586</v>
@@ -1671,56 +1140,56 @@
       <c r="E4" s="19">
         <v>929</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>62</v>
+      <c r="F4" s="19">
+        <v>10.7</v>
       </c>
       <c r="G4" s="19">
         <v>859</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>63</v>
+      <c r="H4" s="18">
+        <v>7.19</v>
       </c>
       <c r="I4" s="18">
         <v>856</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>64</v>
+      <c r="J4" s="18">
+        <v>16.079999999999998</v>
       </c>
       <c r="K4" s="18">
         <v>859</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>65</v>
+      <c r="L4" s="18">
+        <v>2.06</v>
       </c>
       <c r="M4" s="18">
         <v>936</v>
       </c>
-      <c r="N4" s="18" t="s">
-        <v>66</v>
+      <c r="N4" s="18">
+        <v>47.44</v>
       </c>
       <c r="O4" s="18">
         <v>971</v>
       </c>
-      <c r="P4" s="18" t="s">
-        <v>67</v>
+      <c r="P4" s="18">
+        <v>14.03</v>
       </c>
       <c r="Q4" s="18">
         <v>849</v>
       </c>
-      <c r="R4" s="18" t="s">
-        <v>68</v>
+      <c r="R4" s="18">
+        <v>48.95</v>
       </c>
       <c r="S4" s="18">
         <v>910</v>
       </c>
-      <c r="T4" s="18" t="s">
-        <v>69</v>
+      <c r="T4" s="18">
+        <v>5</v>
       </c>
       <c r="U4" s="18">
         <v>735</v>
       </c>
-      <c r="V4" s="18" t="s">
-        <v>70</v>
+      <c r="V4" s="18">
+        <v>59.84</v>
       </c>
       <c r="W4" s="18">
         <v>682</v>
@@ -1729,7 +1198,7 @@
         <v>3.237037037037037E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -1745,56 +1214,56 @@
       <c r="E5" s="19">
         <v>867</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>71</v>
+      <c r="F5" s="19">
+        <v>10.97</v>
       </c>
       <c r="G5" s="19">
         <v>874</v>
       </c>
-      <c r="H5" s="18" t="s">
-        <v>72</v>
+      <c r="H5" s="18">
+        <v>7.25</v>
       </c>
       <c r="I5" s="18">
         <v>882</v>
       </c>
-      <c r="J5" s="18" t="s">
-        <v>73</v>
+      <c r="J5" s="18">
+        <v>16.489999999999998</v>
       </c>
       <c r="K5" s="18">
         <v>915</v>
       </c>
-      <c r="L5" s="18" t="s">
-        <v>46</v>
+      <c r="L5" s="18">
+        <v>2.12</v>
       </c>
       <c r="M5" s="18">
         <v>815</v>
       </c>
-      <c r="N5" s="18" t="s">
-        <v>74</v>
+      <c r="N5" s="18">
+        <v>50</v>
       </c>
       <c r="O5" s="18">
         <v>879</v>
       </c>
-      <c r="P5" s="18" t="s">
-        <v>75</v>
+      <c r="P5" s="18">
+        <v>14.76</v>
       </c>
       <c r="Q5" s="18">
         <v>842</v>
       </c>
-      <c r="R5" s="18" t="s">
-        <v>76</v>
+      <c r="R5" s="18">
+        <v>48.62</v>
       </c>
       <c r="S5" s="18">
         <v>910</v>
       </c>
-      <c r="T5" s="18" t="s">
-        <v>69</v>
+      <c r="T5" s="18">
+        <v>5</v>
       </c>
       <c r="U5" s="18">
         <v>791</v>
       </c>
-      <c r="V5" s="18" t="s">
-        <v>77</v>
+      <c r="V5" s="18">
+        <v>63.51</v>
       </c>
       <c r="W5" s="18">
         <v>700</v>
@@ -1803,7 +1272,7 @@
         <v>3.2052083333333329E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>5</v>
       </c>
@@ -1819,56 +1288,56 @@
       <c r="E6" s="19">
         <v>834</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>78</v>
+      <c r="F6" s="19">
+        <v>11.12</v>
       </c>
       <c r="G6" s="19">
         <v>915</v>
       </c>
-      <c r="H6" s="18" t="s">
-        <v>79</v>
+      <c r="H6" s="18">
+        <v>7.42</v>
       </c>
       <c r="I6" s="18">
         <v>736</v>
       </c>
-      <c r="J6" s="18" t="s">
-        <v>80</v>
+      <c r="J6" s="18">
+        <v>14.12</v>
       </c>
       <c r="K6" s="18">
         <v>859</v>
       </c>
-      <c r="L6" s="18" t="s">
-        <v>65</v>
+      <c r="L6" s="18">
+        <v>2.06</v>
       </c>
       <c r="M6" s="18">
         <v>842</v>
       </c>
-      <c r="N6" s="18" t="s">
-        <v>81</v>
+      <c r="N6" s="18">
+        <v>49.4</v>
       </c>
       <c r="O6" s="18">
         <v>910</v>
       </c>
-      <c r="P6" s="18" t="s">
-        <v>82</v>
+      <c r="P6" s="18">
+        <v>14.51</v>
       </c>
       <c r="Q6" s="18">
         <v>756</v>
       </c>
-      <c r="R6" s="18" t="s">
-        <v>83</v>
+      <c r="R6" s="18">
+        <v>44.48</v>
       </c>
       <c r="S6" s="18">
         <v>1004</v>
       </c>
-      <c r="T6" s="18" t="s">
-        <v>84</v>
+      <c r="T6" s="18">
+        <v>5.3</v>
       </c>
       <c r="U6" s="18">
         <v>787</v>
       </c>
-      <c r="V6" s="18" t="s">
-        <v>85</v>
+      <c r="V6" s="18">
+        <v>63.28</v>
       </c>
       <c r="W6" s="18">
         <v>728</v>
@@ -1877,12 +1346,12 @@
         <v>3.1539351851851854E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17">
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>229</v>
+        <v>52</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>32</v>
@@ -1893,56 +1362,56 @@
       <c r="E7" s="19">
         <v>906</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>86</v>
+      <c r="F7" s="19">
+        <v>10.8</v>
       </c>
       <c r="G7" s="19">
         <v>816</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>87</v>
+      <c r="H7" s="18">
+        <v>7.01</v>
       </c>
       <c r="I7" s="18">
         <v>861</v>
       </c>
-      <c r="J7" s="18" t="s">
-        <v>88</v>
+      <c r="J7" s="18">
+        <v>16.16</v>
       </c>
       <c r="K7" s="18">
         <v>831</v>
       </c>
-      <c r="L7" s="18" t="s">
-        <v>89</v>
+      <c r="L7" s="18">
+        <v>2.0299999999999998</v>
       </c>
       <c r="M7" s="18">
         <v>889</v>
       </c>
-      <c r="N7" s="18" t="s">
-        <v>90</v>
+      <c r="N7" s="18">
+        <v>48.42</v>
       </c>
       <c r="O7" s="18">
         <v>900</v>
       </c>
-      <c r="P7" s="18" t="s">
-        <v>91</v>
+      <c r="P7" s="18">
+        <v>14.59</v>
       </c>
       <c r="Q7" s="18">
         <v>865</v>
       </c>
-      <c r="R7" s="18" t="s">
-        <v>92</v>
+      <c r="R7" s="18">
+        <v>49.76</v>
       </c>
       <c r="S7" s="18">
         <v>880</v>
       </c>
-      <c r="T7" s="18" t="s">
-        <v>93</v>
+      <c r="T7" s="18">
+        <v>4.9000000000000004</v>
       </c>
       <c r="U7" s="18">
         <v>704</v>
       </c>
-      <c r="V7" s="18" t="s">
-        <v>94</v>
+      <c r="V7" s="18">
+        <v>57.75</v>
       </c>
       <c r="W7" s="18">
         <v>705</v>
@@ -1951,7 +1420,7 @@
         <v>3.1962962962962965E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>7</v>
       </c>
@@ -1967,56 +1436,56 @@
       <c r="E8" s="19">
         <v>782</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>95</v>
+      <c r="F8" s="19">
+        <v>11.36</v>
       </c>
       <c r="G8" s="19">
         <v>845</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>96</v>
+      <c r="H8" s="18">
+        <v>7.13</v>
       </c>
       <c r="I8" s="18">
         <v>792</v>
       </c>
-      <c r="J8" s="18" t="s">
-        <v>97</v>
+      <c r="J8" s="18">
+        <v>15.03</v>
       </c>
       <c r="K8" s="18">
         <v>803</v>
       </c>
-      <c r="L8" s="18" t="s">
-        <v>98</v>
+      <c r="L8" s="18">
+        <v>2</v>
       </c>
       <c r="M8" s="18">
         <v>846</v>
       </c>
-      <c r="N8" s="18" t="s">
-        <v>99</v>
+      <c r="N8" s="18">
+        <v>49.32</v>
       </c>
       <c r="O8" s="18">
         <v>929</v>
       </c>
-      <c r="P8" s="18" t="s">
-        <v>100</v>
+      <c r="P8" s="18">
+        <v>14.36</v>
       </c>
       <c r="Q8" s="18">
         <v>757</v>
       </c>
-      <c r="R8" s="18" t="s">
-        <v>101</v>
+      <c r="R8" s="18">
+        <v>44.51</v>
       </c>
       <c r="S8" s="18">
         <v>910</v>
       </c>
-      <c r="T8" s="18" t="s">
-        <v>69</v>
+      <c r="T8" s="18">
+        <v>5</v>
       </c>
       <c r="U8" s="18">
         <v>825</v>
       </c>
-      <c r="V8" s="18" t="s">
-        <v>102</v>
+      <c r="V8" s="18">
+        <v>65.739999999999995</v>
       </c>
       <c r="W8" s="18">
         <v>773</v>
@@ -2025,15 +1494,15 @@
         <v>3.0758101851851849E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17">
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>230</v>
+        <v>53</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="D9" s="19">
         <v>8257</v>
@@ -2041,56 +1510,56 @@
       <c r="E9" s="19">
         <v>922</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>104</v>
+      <c r="F9" s="19">
+        <v>10.73</v>
       </c>
       <c r="G9" s="19">
         <v>850</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>105</v>
+      <c r="H9" s="18">
+        <v>7.15</v>
       </c>
       <c r="I9" s="18">
         <v>786</v>
       </c>
-      <c r="J9" s="18" t="s">
-        <v>106</v>
+      <c r="J9" s="18">
+        <v>14.94</v>
       </c>
       <c r="K9" s="18">
         <v>887</v>
       </c>
-      <c r="L9" s="18" t="s">
-        <v>107</v>
+      <c r="L9" s="18">
+        <v>2.09</v>
       </c>
       <c r="M9" s="18">
         <v>849</v>
       </c>
-      <c r="N9" s="18" t="s">
-        <v>108</v>
+      <c r="N9" s="18">
+        <v>49.25</v>
       </c>
       <c r="O9" s="18">
         <v>964</v>
       </c>
-      <c r="P9" s="18" t="s">
-        <v>109</v>
+      <c r="P9" s="18">
+        <v>14.08</v>
       </c>
       <c r="Q9" s="18">
         <v>724</v>
       </c>
-      <c r="R9" s="18" t="s">
-        <v>110</v>
+      <c r="R9" s="18">
+        <v>42.91</v>
       </c>
       <c r="S9" s="18">
         <v>819</v>
       </c>
-      <c r="T9" s="18" t="s">
-        <v>111</v>
+      <c r="T9" s="18">
+        <v>4.7</v>
       </c>
       <c r="U9" s="18">
         <v>870</v>
       </c>
-      <c r="V9" s="18" t="s">
-        <v>112</v>
+      <c r="V9" s="18">
+        <v>68.739999999999995</v>
       </c>
       <c r="W9" s="18">
         <v>586</v>
@@ -2099,12 +1568,12 @@
         <v>3.4192129629629629E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>231</v>
+        <v>54</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>31</v>
@@ -2115,56 +1584,56 @@
       <c r="E10" s="19">
         <v>890</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>113</v>
+      <c r="F10" s="19">
+        <v>10.87</v>
       </c>
       <c r="G10" s="19">
         <v>854</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>114</v>
+      <c r="H10" s="18">
+        <v>7.17</v>
       </c>
       <c r="I10" s="18">
         <v>703</v>
       </c>
-      <c r="J10" s="18" t="s">
-        <v>115</v>
+      <c r="J10" s="18">
+        <v>13.58</v>
       </c>
       <c r="K10" s="18">
         <v>803</v>
       </c>
-      <c r="L10" s="18" t="s">
-        <v>98</v>
+      <c r="L10" s="18">
+        <v>2</v>
       </c>
       <c r="M10" s="18">
         <v>881</v>
       </c>
-      <c r="N10" s="18" t="s">
-        <v>116</v>
+      <c r="N10" s="18">
+        <v>48.58</v>
       </c>
       <c r="O10" s="18">
         <v>985</v>
       </c>
-      <c r="P10" s="18" t="s">
-        <v>117</v>
+      <c r="P10" s="18">
+        <v>13.92</v>
       </c>
       <c r="Q10" s="18">
         <v>691</v>
       </c>
-      <c r="R10" s="18" t="s">
-        <v>118</v>
+      <c r="R10" s="18">
+        <v>41.28</v>
       </c>
       <c r="S10" s="18">
         <v>819</v>
       </c>
-      <c r="T10" s="18" t="s">
-        <v>111</v>
+      <c r="T10" s="18">
+        <v>4.7</v>
       </c>
       <c r="U10" s="18">
         <v>817</v>
       </c>
-      <c r="V10" s="18" t="s">
-        <v>119</v>
+      <c r="V10" s="18">
+        <v>65.239999999999995</v>
       </c>
       <c r="W10" s="18">
         <v>800</v>
@@ -2173,7 +1642,7 @@
         <v>3.0288194444444447E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>10</v>
       </c>
@@ -2189,56 +1658,56 @@
       <c r="E11" s="19">
         <v>872</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>120</v>
+      <c r="F11" s="19">
+        <v>10.95</v>
       </c>
       <c r="G11" s="19">
         <v>876</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>121</v>
+      <c r="H11" s="18">
+        <v>7.26</v>
       </c>
       <c r="I11" s="18">
         <v>778</v>
       </c>
-      <c r="J11" s="18" t="s">
-        <v>122</v>
+      <c r="J11" s="18">
+        <v>14.81</v>
       </c>
       <c r="K11" s="18">
         <v>803</v>
       </c>
-      <c r="L11" s="18" t="s">
-        <v>98</v>
+      <c r="L11" s="18">
+        <v>2</v>
       </c>
       <c r="M11" s="18">
         <v>845</v>
       </c>
-      <c r="N11" s="18" t="s">
-        <v>123</v>
+      <c r="N11" s="18">
+        <v>49.34</v>
       </c>
       <c r="O11" s="18">
         <v>837</v>
       </c>
-      <c r="P11" s="18" t="s">
-        <v>124</v>
+      <c r="P11" s="18">
+        <v>15.1</v>
       </c>
       <c r="Q11" s="18">
         <v>763</v>
       </c>
-      <c r="R11" s="18" t="s">
-        <v>125</v>
+      <c r="R11" s="18">
+        <v>44.81</v>
       </c>
       <c r="S11" s="18">
         <v>972</v>
       </c>
-      <c r="T11" s="18" t="s">
-        <v>126</v>
+      <c r="T11" s="18">
+        <v>5.2</v>
       </c>
       <c r="U11" s="18">
         <v>677</v>
       </c>
-      <c r="V11" s="18" t="s">
-        <v>127</v>
+      <c r="V11" s="18">
+        <v>55.96</v>
       </c>
       <c r="W11" s="18">
         <v>697</v>
@@ -2247,12 +1716,12 @@
         <v>3.210416666666667E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17">
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>232</v>
+        <v>55</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>41</v>
@@ -2263,56 +1732,56 @@
       <c r="E12" s="19">
         <v>836</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>128</v>
+      <c r="F12" s="19">
+        <v>11.11</v>
       </c>
       <c r="G12" s="19">
         <v>898</v>
       </c>
-      <c r="H12" s="18" t="s">
-        <v>129</v>
+      <c r="H12" s="18">
+        <v>7.35</v>
       </c>
       <c r="I12" s="18">
         <v>769</v>
       </c>
-      <c r="J12" s="18" t="s">
-        <v>130</v>
+      <c r="J12" s="18">
+        <v>14.67</v>
       </c>
       <c r="K12" s="18">
         <v>696</v>
       </c>
-      <c r="L12" s="18" t="s">
-        <v>131</v>
+      <c r="L12" s="18">
+        <v>1.88</v>
       </c>
       <c r="M12" s="18">
         <v>884</v>
       </c>
-      <c r="N12" s="18" t="s">
-        <v>132</v>
+      <c r="N12" s="18">
+        <v>48.52</v>
       </c>
       <c r="O12" s="18">
         <v>878</v>
       </c>
-      <c r="P12" s="18" t="s">
-        <v>133</v>
+      <c r="P12" s="18">
+        <v>14.77</v>
       </c>
       <c r="Q12" s="18">
         <v>752</v>
       </c>
-      <c r="R12" s="18" t="s">
-        <v>134</v>
+      <c r="R12" s="18">
+        <v>44.3</v>
       </c>
       <c r="S12" s="18">
         <v>702</v>
       </c>
-      <c r="T12" s="18" t="s">
-        <v>135</v>
+      <c r="T12" s="18">
+        <v>4.3</v>
       </c>
       <c r="U12" s="18">
         <v>824</v>
       </c>
-      <c r="V12" s="18" t="s">
-        <v>136</v>
+      <c r="V12" s="18">
+        <v>65.709999999999994</v>
       </c>
       <c r="W12" s="18">
         <v>795</v>
@@ -2321,7 +1790,7 @@
         <v>3.0381944444444445E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17">
         <v>12</v>
       </c>
@@ -2337,56 +1806,56 @@
       <c r="E13" s="19">
         <v>765</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>137</v>
+      <c r="F13" s="19">
+        <v>11.44</v>
       </c>
       <c r="G13" s="19">
         <v>814</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>138</v>
+      <c r="H13" s="18">
+        <v>7</v>
       </c>
       <c r="I13" s="18">
         <v>798</v>
       </c>
-      <c r="J13" s="18" t="s">
-        <v>139</v>
+      <c r="J13" s="18">
+        <v>15.13</v>
       </c>
       <c r="K13" s="18">
         <v>887</v>
       </c>
-      <c r="L13" s="18" t="s">
-        <v>107</v>
+      <c r="L13" s="18">
+        <v>2.09</v>
       </c>
       <c r="M13" s="18">
         <v>788</v>
       </c>
-      <c r="N13" s="18" t="s">
-        <v>140</v>
+      <c r="N13" s="18">
+        <v>50.58</v>
       </c>
       <c r="O13" s="18">
         <v>871</v>
       </c>
-      <c r="P13" s="18" t="s">
-        <v>141</v>
+      <c r="P13" s="18">
+        <v>14.82</v>
       </c>
       <c r="Q13" s="18">
         <v>804</v>
       </c>
-      <c r="R13" s="18" t="s">
-        <v>142</v>
+      <c r="R13" s="18">
+        <v>46.8</v>
       </c>
       <c r="S13" s="18">
         <v>849</v>
       </c>
-      <c r="T13" s="18" t="s">
-        <v>50</v>
+      <c r="T13" s="18">
+        <v>4.8</v>
       </c>
       <c r="U13" s="18">
         <v>732</v>
       </c>
-      <c r="V13" s="18" t="s">
-        <v>143</v>
+      <c r="V13" s="18">
+        <v>59.63</v>
       </c>
       <c r="W13" s="18">
         <v>709</v>
@@ -2395,12 +1864,12 @@
         <v>3.1892361111111114E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>233</v>
+        <v>56</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>24</v>
@@ -2411,56 +1880,56 @@
       <c r="E14" s="19">
         <v>830</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>144</v>
+      <c r="F14" s="19">
+        <v>11.14</v>
       </c>
       <c r="G14" s="19">
         <v>781</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>145</v>
+      <c r="H14" s="18">
+        <v>6.86</v>
       </c>
       <c r="I14" s="18">
         <v>773</v>
       </c>
-      <c r="J14" s="18" t="s">
-        <v>146</v>
+      <c r="J14" s="18">
+        <v>14.73</v>
       </c>
       <c r="K14" s="18">
         <v>859</v>
       </c>
-      <c r="L14" s="18" t="s">
-        <v>65</v>
+      <c r="L14" s="18">
+        <v>2.06</v>
       </c>
       <c r="M14" s="18">
         <v>860</v>
       </c>
-      <c r="N14" s="18" t="s">
-        <v>147</v>
+      <c r="N14" s="18">
+        <v>49.02</v>
       </c>
       <c r="O14" s="18">
         <v>884</v>
       </c>
-      <c r="P14" s="18" t="s">
-        <v>148</v>
+      <c r="P14" s="18">
+        <v>14.72</v>
       </c>
       <c r="Q14" s="18">
         <v>740</v>
       </c>
-      <c r="R14" s="18" t="s">
-        <v>149</v>
+      <c r="R14" s="18">
+        <v>43.7</v>
       </c>
       <c r="S14" s="18">
         <v>941</v>
       </c>
-      <c r="T14" s="18" t="s">
-        <v>150</v>
+      <c r="T14" s="18">
+        <v>5.0999999999999996</v>
       </c>
       <c r="U14" s="18">
         <v>678</v>
       </c>
-      <c r="V14" s="18" t="s">
-        <v>151</v>
+      <c r="V14" s="18">
+        <v>56.01</v>
       </c>
       <c r="W14" s="18">
         <v>658</v>
@@ -2469,15 +1938,15 @@
         <v>3.2821759259259258E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17">
         <v>14</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>234</v>
+        <v>57</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
       <c r="D15" s="19">
         <v>7984</v>
@@ -2485,56 +1954,56 @@
       <c r="E15" s="19">
         <v>797</v>
       </c>
-      <c r="F15" s="19" t="s">
-        <v>153</v>
+      <c r="F15" s="19">
+        <v>11.29</v>
       </c>
       <c r="G15" s="19">
         <v>795</v>
       </c>
-      <c r="H15" s="18" t="s">
-        <v>154</v>
+      <c r="H15" s="18">
+        <v>6.92</v>
       </c>
       <c r="I15" s="18">
         <v>850</v>
       </c>
-      <c r="J15" s="18" t="s">
-        <v>155</v>
+      <c r="J15" s="18">
+        <v>15.98</v>
       </c>
       <c r="K15" s="18">
         <v>749</v>
       </c>
-      <c r="L15" s="18" t="s">
-        <v>156</v>
+      <c r="L15" s="18">
+        <v>1.94</v>
       </c>
       <c r="M15" s="18">
         <v>762</v>
       </c>
-      <c r="N15" s="18" t="s">
-        <v>157</v>
+      <c r="N15" s="18">
+        <v>51.16</v>
       </c>
       <c r="O15" s="18">
         <v>858</v>
       </c>
-      <c r="P15" s="18" t="s">
-        <v>158</v>
+      <c r="P15" s="18">
+        <v>14.93</v>
       </c>
       <c r="Q15" s="18">
         <v>764</v>
       </c>
-      <c r="R15" s="18" t="s">
-        <v>159</v>
+      <c r="R15" s="18">
+        <v>44.86</v>
       </c>
       <c r="S15" s="18">
         <v>819</v>
       </c>
-      <c r="T15" s="18" t="s">
-        <v>111</v>
+      <c r="T15" s="18">
+        <v>4.7</v>
       </c>
       <c r="U15" s="18">
         <v>876</v>
       </c>
-      <c r="V15" s="18" t="s">
-        <v>160</v>
+      <c r="V15" s="18">
+        <v>69.14</v>
       </c>
       <c r="W15" s="18">
         <v>714</v>
@@ -2543,12 +2012,12 @@
         <v>3.1785879629629629E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17">
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>235</v>
+        <v>58</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>41</v>
@@ -2559,56 +2028,56 @@
       <c r="E16" s="19">
         <v>935</v>
       </c>
-      <c r="F16" s="19" t="s">
-        <v>161</v>
+      <c r="F16" s="19">
+        <v>10.67</v>
       </c>
       <c r="G16" s="19">
         <v>850</v>
       </c>
-      <c r="H16" s="18" t="s">
-        <v>105</v>
+      <c r="H16" s="18">
+        <v>7.15</v>
       </c>
       <c r="I16" s="18">
         <v>712</v>
       </c>
-      <c r="J16" s="18" t="s">
-        <v>162</v>
+      <c r="J16" s="18">
+        <v>13.74</v>
       </c>
       <c r="K16" s="18">
         <v>670</v>
       </c>
-      <c r="L16" s="18" t="s">
-        <v>163</v>
+      <c r="L16" s="18">
+        <v>1.85</v>
       </c>
       <c r="M16" s="18">
         <v>910</v>
       </c>
-      <c r="N16" s="18" t="s">
-        <v>164</v>
+      <c r="N16" s="18">
+        <v>47.98</v>
       </c>
       <c r="O16" s="18">
         <v>847</v>
       </c>
-      <c r="P16" s="18" t="s">
-        <v>165</v>
+      <c r="P16" s="18">
+        <v>15.02</v>
       </c>
       <c r="Q16" s="18">
         <v>662</v>
       </c>
-      <c r="R16" s="18" t="s">
-        <v>166</v>
+      <c r="R16" s="18">
+        <v>39.869999999999997</v>
       </c>
       <c r="S16" s="18">
         <v>910</v>
       </c>
-      <c r="T16" s="18" t="s">
-        <v>69</v>
+      <c r="T16" s="18">
+        <v>5</v>
       </c>
       <c r="U16" s="18">
         <v>704</v>
       </c>
-      <c r="V16" s="18" t="s">
-        <v>167</v>
+      <c r="V16" s="18">
+        <v>57.73</v>
       </c>
       <c r="W16" s="18">
         <v>774</v>
@@ -2617,12 +2086,12 @@
         <v>3.0730324074074076E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>236</v>
+        <v>59</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>38</v>
@@ -2633,56 +2102,56 @@
       <c r="E17" s="19">
         <v>878</v>
       </c>
-      <c r="F17" s="19" t="s">
-        <v>168</v>
+      <c r="F17" s="19">
+        <v>10.92</v>
       </c>
       <c r="G17" s="19">
         <v>915</v>
       </c>
-      <c r="H17" s="18" t="s">
-        <v>79</v>
+      <c r="H17" s="18">
+        <v>7.42</v>
       </c>
       <c r="I17" s="18">
         <v>744</v>
       </c>
-      <c r="J17" s="18" t="s">
-        <v>169</v>
+      <c r="J17" s="18">
+        <v>14.26</v>
       </c>
       <c r="K17" s="18">
         <v>670</v>
       </c>
-      <c r="L17" s="18" t="s">
-        <v>163</v>
+      <c r="L17" s="18">
+        <v>1.85</v>
       </c>
       <c r="M17" s="18">
         <v>866</v>
       </c>
-      <c r="N17" s="18" t="s">
-        <v>170</v>
+      <c r="N17" s="18">
+        <v>48.89</v>
       </c>
       <c r="O17" s="18">
         <v>910</v>
       </c>
-      <c r="P17" s="18" t="s">
-        <v>82</v>
+      <c r="P17" s="18">
+        <v>14.51</v>
       </c>
       <c r="Q17" s="18">
         <v>605</v>
       </c>
-      <c r="R17" s="18" t="s">
-        <v>171</v>
+      <c r="R17" s="18">
+        <v>37.07</v>
       </c>
       <c r="S17" s="18">
         <v>819</v>
       </c>
-      <c r="T17" s="18" t="s">
-        <v>111</v>
+      <c r="T17" s="18">
+        <v>4.7</v>
       </c>
       <c r="U17" s="18">
         <v>743</v>
       </c>
-      <c r="V17" s="18" t="s">
-        <v>172</v>
+      <c r="V17" s="18">
+        <v>60.34</v>
       </c>
       <c r="W17" s="18">
         <v>644</v>
@@ -2691,12 +2160,12 @@
         <v>3.3082175925925922E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17">
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>237</v>
+        <v>60</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>42</v>
@@ -2707,56 +2176,56 @@
       <c r="E18" s="19">
         <v>823</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>173</v>
+      <c r="F18" s="19">
+        <v>11.17</v>
       </c>
       <c r="G18" s="19">
         <v>842</v>
       </c>
-      <c r="H18" s="18" t="s">
-        <v>174</v>
+      <c r="H18" s="18">
+        <v>7.12</v>
       </c>
       <c r="I18" s="18">
         <v>685</v>
       </c>
-      <c r="J18" s="18" t="s">
-        <v>175</v>
+      <c r="J18" s="18">
+        <v>13.29</v>
       </c>
       <c r="K18" s="18">
         <v>831</v>
       </c>
-      <c r="L18" s="18" t="s">
-        <v>89</v>
+      <c r="L18" s="18">
+        <v>2.0299999999999998</v>
       </c>
       <c r="M18" s="18">
         <v>721</v>
       </c>
-      <c r="N18" s="18" t="s">
-        <v>176</v>
+      <c r="N18" s="18">
+        <v>52.08</v>
       </c>
       <c r="O18" s="18">
         <v>880</v>
       </c>
-      <c r="P18" s="18" t="s">
-        <v>177</v>
+      <c r="P18" s="18">
+        <v>14.75</v>
       </c>
       <c r="Q18" s="18">
         <v>740</v>
       </c>
-      <c r="R18" s="18" t="s">
-        <v>178</v>
+      <c r="R18" s="18">
+        <v>43.67</v>
       </c>
       <c r="S18" s="18">
         <v>910</v>
       </c>
-      <c r="T18" s="18" t="s">
-        <v>69</v>
+      <c r="T18" s="18">
+        <v>5</v>
       </c>
       <c r="U18" s="18">
         <v>688</v>
       </c>
-      <c r="V18" s="18" t="s">
-        <v>179</v>
+      <c r="V18" s="18">
+        <v>56.69</v>
       </c>
       <c r="W18" s="18">
         <v>629</v>
@@ -2765,15 +2234,15 @@
         <v>3.3364583333333332E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17">
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>238</v>
+        <v>61</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="D19" s="19">
         <v>7657</v>
@@ -2781,56 +2250,56 @@
       <c r="E19" s="19">
         <v>832</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>180</v>
+      <c r="F19" s="19">
+        <v>11.13</v>
       </c>
       <c r="G19" s="19">
         <v>918</v>
       </c>
-      <c r="H19" s="18" t="s">
-        <v>181</v>
+      <c r="H19" s="18">
+        <v>7.43</v>
       </c>
       <c r="I19" s="18">
         <v>700</v>
       </c>
-      <c r="J19" s="18" t="s">
-        <v>182</v>
+      <c r="J19" s="18">
+        <v>13.54</v>
       </c>
       <c r="K19" s="18">
         <v>887</v>
       </c>
-      <c r="L19" s="18" t="s">
-        <v>107</v>
+      <c r="L19" s="18">
+        <v>2.09</v>
       </c>
       <c r="M19" s="18">
         <v>798</v>
       </c>
-      <c r="N19" s="18" t="s">
-        <v>183</v>
+      <c r="N19" s="18">
+        <v>50.37</v>
       </c>
       <c r="O19" s="18">
         <v>853</v>
       </c>
-      <c r="P19" s="18" t="s">
-        <v>184</v>
+      <c r="P19" s="18">
+        <v>14.97</v>
       </c>
       <c r="Q19" s="18">
         <v>699</v>
       </c>
-      <c r="R19" s="18" t="s">
-        <v>185</v>
+      <c r="R19" s="18">
+        <v>41.69</v>
       </c>
       <c r="S19" s="18">
         <v>673</v>
       </c>
-      <c r="T19" s="18" t="s">
-        <v>186</v>
+      <c r="T19" s="18">
+        <v>4.2</v>
       </c>
       <c r="U19" s="18">
         <v>682</v>
       </c>
-      <c r="V19" s="18" t="s">
-        <v>187</v>
+      <c r="V19" s="18">
+        <v>56.28</v>
       </c>
       <c r="W19" s="18">
         <v>615</v>
@@ -2839,15 +2308,15 @@
         <v>3.3644675925925929E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17">
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>239</v>
+        <v>62</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>188</v>
+        <v>47</v>
       </c>
       <c r="D20" s="19">
         <v>7629</v>
@@ -2855,56 +2324,56 @@
       <c r="E20" s="19">
         <v>850</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>189</v>
+      <c r="F20" s="19">
+        <v>11.05</v>
       </c>
       <c r="G20" s="19">
         <v>762</v>
       </c>
-      <c r="H20" s="18" t="s">
-        <v>190</v>
+      <c r="H20" s="18">
+        <v>6.78</v>
       </c>
       <c r="I20" s="18">
         <v>602</v>
       </c>
-      <c r="J20" s="18" t="s">
-        <v>191</v>
+      <c r="J20" s="18">
+        <v>11.92</v>
       </c>
       <c r="K20" s="18">
         <v>696</v>
       </c>
-      <c r="L20" s="18" t="s">
-        <v>131</v>
+      <c r="L20" s="18">
+        <v>1.88</v>
       </c>
       <c r="M20" s="18">
         <v>881</v>
       </c>
-      <c r="N20" s="18" t="s">
-        <v>192</v>
+      <c r="N20" s="18">
+        <v>48.59</v>
       </c>
       <c r="O20" s="18">
         <v>787</v>
       </c>
-      <c r="P20" s="18" t="s">
-        <v>193</v>
+      <c r="P20" s="18">
+        <v>15.53</v>
       </c>
       <c r="Q20" s="18">
         <v>698</v>
       </c>
-      <c r="R20" s="18" t="s">
-        <v>194</v>
+      <c r="R20" s="18">
+        <v>41.65</v>
       </c>
       <c r="S20" s="18">
         <v>941</v>
       </c>
-      <c r="T20" s="18" t="s">
-        <v>150</v>
+      <c r="T20" s="18">
+        <v>5.0999999999999996</v>
       </c>
       <c r="U20" s="18">
         <v>732</v>
       </c>
-      <c r="V20" s="18" t="s">
-        <v>195</v>
+      <c r="V20" s="18">
+        <v>59.59</v>
       </c>
       <c r="W20" s="18">
         <v>680</v>
@@ -2913,12 +2382,12 @@
         <v>3.241203703703704E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17">
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>240</v>
+        <v>63</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>26</v>
@@ -2929,56 +2398,56 @@
       <c r="E21" s="19">
         <v>834</v>
       </c>
-      <c r="F21" s="19" t="s">
-        <v>78</v>
+      <c r="F21" s="19">
+        <v>11.12</v>
       </c>
       <c r="G21" s="19">
         <v>920</v>
       </c>
-      <c r="H21" s="18" t="s">
-        <v>196</v>
+      <c r="H21" s="18">
+        <v>7.44</v>
       </c>
       <c r="I21" s="18">
         <v>681</v>
       </c>
-      <c r="J21" s="18" t="s">
-        <v>197</v>
+      <c r="J21" s="18">
+        <v>13.23</v>
       </c>
       <c r="K21" s="18">
         <v>749</v>
       </c>
-      <c r="L21" s="18" t="s">
-        <v>156</v>
+      <c r="L21" s="18">
+        <v>1.94</v>
       </c>
       <c r="M21" s="18">
         <v>787</v>
       </c>
-      <c r="N21" s="18" t="s">
-        <v>198</v>
+      <c r="N21" s="18">
+        <v>50.6</v>
       </c>
       <c r="O21" s="18">
         <v>829</v>
       </c>
-      <c r="P21" s="18" t="s">
-        <v>199</v>
+      <c r="P21" s="18">
+        <v>15.17</v>
       </c>
       <c r="Q21" s="18">
         <v>779</v>
       </c>
-      <c r="R21" s="18" t="s">
-        <v>200</v>
+      <c r="R21" s="18">
+        <v>45.58</v>
       </c>
       <c r="S21" s="18">
         <v>731</v>
       </c>
-      <c r="T21" s="18" t="s">
-        <v>201</v>
+      <c r="T21" s="18">
+        <v>4.4000000000000004</v>
       </c>
       <c r="U21" s="18">
         <v>578</v>
       </c>
-      <c r="V21" s="18" t="s">
-        <v>202</v>
+      <c r="V21" s="18">
+        <v>49.28</v>
       </c>
       <c r="W21" s="18">
         <v>737</v>
@@ -2987,15 +2456,15 @@
         <v>3.1390046296296292E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <v>21</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>241</v>
+        <v>64</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>203</v>
+        <v>48</v>
       </c>
       <c r="D22" s="19">
         <v>7531</v>
@@ -3003,56 +2472,56 @@
       <c r="E22" s="19">
         <v>797</v>
       </c>
-      <c r="F22" s="19" t="s">
-        <v>153</v>
+      <c r="F22" s="19">
+        <v>11.29</v>
       </c>
       <c r="G22" s="19">
         <v>842</v>
       </c>
-      <c r="H22" s="18" t="s">
-        <v>174</v>
+      <c r="H22" s="18">
+        <v>7.12</v>
       </c>
       <c r="I22" s="18">
         <v>657</v>
       </c>
-      <c r="J22" s="18" t="s">
-        <v>204</v>
+      <c r="J22" s="18">
+        <v>12.83</v>
       </c>
       <c r="K22" s="18">
         <v>723</v>
       </c>
-      <c r="L22" s="18" t="s">
-        <v>205</v>
+      <c r="L22" s="18">
+        <v>1.91</v>
       </c>
       <c r="M22" s="18">
         <v>862</v>
       </c>
-      <c r="N22" s="18" t="s">
-        <v>206</v>
+      <c r="N22" s="18">
+        <v>48.99</v>
       </c>
       <c r="O22" s="18">
         <v>863</v>
       </c>
-      <c r="P22" s="18" t="s">
-        <v>207</v>
+      <c r="P22" s="18">
+        <v>14.89</v>
       </c>
       <c r="Q22" s="18">
         <v>588</v>
       </c>
-      <c r="R22" s="18" t="s">
-        <v>208</v>
+      <c r="R22" s="18">
+        <v>36.229999999999997</v>
       </c>
       <c r="S22" s="18">
         <v>849</v>
       </c>
-      <c r="T22" s="18" t="s">
-        <v>50</v>
+      <c r="T22" s="18">
+        <v>4.8</v>
       </c>
       <c r="U22" s="18">
         <v>512</v>
       </c>
-      <c r="V22" s="18" t="s">
-        <v>209</v>
+      <c r="V22" s="18">
+        <v>44.79</v>
       </c>
       <c r="W22" s="18">
         <v>838</v>
@@ -3061,12 +2530,12 @@
         <v>2.9648148148148147E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17">
         <v>22</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>242</v>
+        <v>65</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>31</v>
@@ -3077,56 +2546,56 @@
       <c r="E23" s="19">
         <v>883</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>210</v>
+      <c r="F23" s="19">
+        <v>10.9</v>
       </c>
       <c r="G23" s="19">
         <v>920</v>
       </c>
-      <c r="H23" s="18" t="s">
-        <v>196</v>
+      <c r="H23" s="18">
+        <v>7.44</v>
       </c>
       <c r="I23" s="18">
         <v>801</v>
       </c>
-      <c r="J23" s="18" t="s">
-        <v>211</v>
+      <c r="J23" s="18">
+        <v>15.18</v>
       </c>
       <c r="K23" s="18">
         <v>776</v>
       </c>
-      <c r="L23" s="18" t="s">
-        <v>56</v>
+      <c r="L23" s="18">
+        <v>1.97</v>
       </c>
       <c r="M23" s="18">
         <v>930</v>
       </c>
-      <c r="N23" s="18" t="s">
-        <v>212</v>
+      <c r="N23" s="18">
+        <v>47.58</v>
       </c>
       <c r="O23" s="18">
         <v>885</v>
       </c>
-      <c r="P23" s="18" t="s">
-        <v>213</v>
+      <c r="P23" s="18">
+        <v>14.71</v>
       </c>
       <c r="Q23" s="18">
         <v>685</v>
       </c>
-      <c r="R23" s="18" t="s">
-        <v>214</v>
+      <c r="R23" s="18">
+        <v>40.99</v>
       </c>
       <c r="S23" s="18">
         <v>0</v>
       </c>
-      <c r="T23" s="18" t="s">
-        <v>215</v>
+      <c r="T23" s="18">
+        <v>0</v>
       </c>
       <c r="U23" s="18">
         <v>722</v>
       </c>
-      <c r="V23" s="18" t="s">
-        <v>216</v>
+      <c r="V23" s="18">
+        <v>58.93</v>
       </c>
       <c r="W23" s="18">
         <v>742</v>
@@ -3135,15 +2604,15 @@
         <v>3.1293981481481481E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17">
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>243</v>
+        <v>66</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>217</v>
+        <v>49</v>
       </c>
       <c r="D24" s="19">
         <v>6698</v>
@@ -3151,56 +2620,56 @@
       <c r="E24" s="19">
         <v>814</v>
       </c>
-      <c r="F24" s="19" t="s">
-        <v>218</v>
+      <c r="F24" s="19">
+        <v>11.21</v>
       </c>
       <c r="G24" s="19">
         <v>797</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>219</v>
+      <c r="H24" s="18">
+        <v>6.93</v>
       </c>
       <c r="I24" s="18">
         <v>707</v>
       </c>
-      <c r="J24" s="18" t="s">
-        <v>220</v>
+      <c r="J24" s="18">
+        <v>13.65</v>
       </c>
       <c r="K24" s="18">
         <v>644</v>
       </c>
-      <c r="L24" s="18" t="s">
-        <v>221</v>
+      <c r="L24" s="18">
+        <v>1.82</v>
       </c>
       <c r="M24" s="18">
         <v>783</v>
       </c>
-      <c r="N24" s="18" t="s">
-        <v>222</v>
+      <c r="N24" s="18">
+        <v>50.7</v>
       </c>
       <c r="O24" s="18">
         <v>8</v>
       </c>
-      <c r="P24" s="18" t="s">
-        <v>223</v>
+      <c r="P24" s="18">
+        <v>27.24</v>
       </c>
       <c r="Q24" s="18">
         <v>773</v>
       </c>
-      <c r="R24" s="18" t="s">
-        <v>224</v>
+      <c r="R24" s="18">
+        <v>45.31</v>
       </c>
       <c r="S24" s="18">
         <v>760</v>
       </c>
-      <c r="T24" s="18" t="s">
-        <v>225</v>
+      <c r="T24" s="18">
+        <v>4.5</v>
       </c>
       <c r="U24" s="18">
         <v>762</v>
       </c>
-      <c r="V24" s="18" t="s">
-        <v>226</v>
+      <c r="V24" s="18">
+        <v>61.63</v>
       </c>
       <c r="W24" s="18">
         <v>650</v>
@@ -3209,14 +2678,14 @@
         <v>3.2975694444444445E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N26" s="1"/>
       <c r="S26" s="2"/>
     </row>
-    <row r="27" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
       <c r="C27" s="4" t="s">
         <v>27</v>
@@ -3229,7 +2698,7 @@
       </c>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>4</v>
       </c>
@@ -3244,7 +2713,7 @@
       </c>
       <c r="P28" s="14"/>
     </row>
-    <row r="29" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>12</v>
       </c>
@@ -3258,7 +2727,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
@@ -3272,7 +2741,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
@@ -3286,7 +2755,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7" t="s">
         <v>10</v>
       </c>
@@ -3300,7 +2769,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>18</v>
       </c>
@@ -3314,7 +2783,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>6</v>
       </c>
@@ -3328,7 +2797,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>8</v>
       </c>
@@ -3342,7 +2811,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>16</v>
       </c>
@@ -3356,7 +2825,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>20</v>
       </c>
@@ -3370,8 +2839,8 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I39" s="15"/>
     </row>
   </sheetData>

</xml_diff>